<commit_message>
revised with danny corrections on ling's thesis
</commit_message>
<xml_diff>
--- a/results/VIGraphs2.xlsx
+++ b/results/VIGraphs2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="4260" yWindow="0" windowWidth="33700" windowHeight="17580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
   <si>
     <t>Results for ESvES2 copy.txt</t>
   </si>
@@ -201,8 +201,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -238,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -254,6 +274,16 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -269,6 +299,16 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -290,31 +330,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>ES</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs ES2 for nu of 50</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -550,15 +566,15 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090537256"/>
-        <c:axId val="2090617256"/>
+        <c:axId val="2081051816"/>
+        <c:axId val="2081058568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090537256"/>
+        <c:axId val="2081051816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -587,7 +603,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090617256"/>
+        <c:crossAx val="2081058568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -595,7 +611,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090617256"/>
+        <c:axId val="2081058568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090537256"/>
+        <c:crossAx val="2081051816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -670,31 +686,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>All demarcators</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> on nu of 50</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1032,7 +1024,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$N$7</c:f>
+              <c:f>all!$O$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1051,7 +1043,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>all!$N$8:$N$33</c:f>
+              <c:f>all!$O$8:$O$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1143,7 +1135,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$O$7</c:f>
+              <c:f>all!$P$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1157,7 +1149,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>all!$O$8:$O$33</c:f>
+              <c:f>all!$P$8:$P$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1238,6 +1230,109 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>4.21377645808</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>es</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cmpd="sng">
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>all!$N$8:$N$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.673482168912</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.321142609407</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.333886400573</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.37320979706</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.927909278696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4816546708</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.70349809226</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.22894291595</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.15608430732</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.485643205207</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.983387941228</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.30142432336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.23291706212</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.04731588468</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.797618949029</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.37988448326</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.10765021286</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.42062857123</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.616034869164</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.222071124879</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.10751685016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.50631299666</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.18006168118</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.699877060146</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.79223391517</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.8272644064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1254,15 +1349,15 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106092360"/>
-        <c:axId val="2106114264"/>
+        <c:axId val="2081146312"/>
+        <c:axId val="2081152040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106092360"/>
+        <c:axId val="2081146312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1286,7 +1381,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106114264"/>
+        <c:crossAx val="2081152040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1294,7 +1389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106114264"/>
+        <c:axId val="2081152040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,7 +1418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106092360"/>
+        <c:crossAx val="2081146312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1364,26 +1459,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>All demarcators on nu of 100</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1943,15 +2019,15 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2093860408"/>
-        <c:axId val="2105541160"/>
+        <c:axId val="2081195800"/>
+        <c:axId val="2081201512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2093860408"/>
+        <c:axId val="2081195800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1975,7 +2051,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105541160"/>
+        <c:crossAx val="2081201512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1983,7 +2059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105541160"/>
+        <c:axId val="2081201512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,7 +2088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093860408"/>
+        <c:crossAx val="2081195800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2053,26 +2129,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>All demarcators on nu of 200</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -2632,15 +2689,15 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109077336"/>
-        <c:axId val="2094613000"/>
+        <c:axId val="2082937176"/>
+        <c:axId val="2082943160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109077336"/>
+        <c:axId val="2082937176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2669,7 +2726,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094613000"/>
+        <c:crossAx val="2082943160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2677,7 +2734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094613000"/>
+        <c:axId val="2082943160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2706,7 +2763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109077336"/>
+        <c:crossAx val="2082937176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2738,15 +2795,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2767,16 +2824,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2797,16 +2854,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2827,16 +2884,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2863,7 +2920,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nu100" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ESvES2" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2871,7 +2928,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ESvES2" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nu100" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3198,8 +3255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39:X41"/>
+    <sheetView tabSelected="1" topLeftCell="H31" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3271,9 +3328,12 @@
         <v>9</v>
       </c>
       <c r="N7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" t="s">
         <v>5</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>10</v>
       </c>
       <c r="Q7" t="s">
@@ -3360,9 +3420,12 @@
         <v>1.5434762955800001</v>
       </c>
       <c r="N8">
+        <v>0.67348216891199997</v>
+      </c>
+      <c r="O8">
         <v>1.66584191949</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>3.2006092760199998</v>
       </c>
       <c r="Q8">
@@ -3449,9 +3512,12 @@
         <v>1.1858402962300001</v>
       </c>
       <c r="N9">
+        <v>0.32114260940700001</v>
+      </c>
+      <c r="O9">
         <v>1.2699881612399999</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>3.3708421747699999</v>
       </c>
       <c r="Q9">
@@ -3538,9 +3604,12 @@
         <v>0.94823541044000004</v>
       </c>
       <c r="N10">
+        <v>0.33388640057300001</v>
+      </c>
+      <c r="O10">
         <v>1.12481426061</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>3.36158217911</v>
       </c>
       <c r="Q10">
@@ -3627,9 +3696,12 @@
         <v>2.0294836113699999</v>
       </c>
       <c r="N11">
+        <v>1.3732097970599999</v>
+      </c>
+      <c r="O11">
         <v>1.7630128597800001</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>3.5484315039599998</v>
       </c>
       <c r="Q11">
@@ -3716,9 +3788,12 @@
         <v>1.41621593954</v>
       </c>
       <c r="N12">
+        <v>0.92790927869600004</v>
+      </c>
+      <c r="O12">
         <v>1.34363156923</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>2.9914827445399998</v>
       </c>
       <c r="Q12">
@@ -3805,9 +3880,12 @@
         <v>1.1928974993100001</v>
       </c>
       <c r="N13">
+        <v>1.4816546708</v>
+      </c>
+      <c r="O13">
         <v>1.1135870719700001</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>3.1484957320000002</v>
       </c>
       <c r="Q13">
@@ -3894,9 +3972,12 @@
         <v>2.30816356413</v>
       </c>
       <c r="N14">
+        <v>1.70349809226</v>
+      </c>
+      <c r="O14">
         <v>1.9466986770000001</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>3.37516832817</v>
       </c>
       <c r="Q14">
@@ -3983,9 +4064,12 @@
         <v>2.5651541955899999</v>
       </c>
       <c r="N15">
+        <v>2.2289429159499998</v>
+      </c>
+      <c r="O15">
         <v>2.39189073387</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>3.0626803623900001</v>
       </c>
       <c r="Q15">
@@ -4072,9 +4156,12 @@
         <v>1.64003801727</v>
       </c>
       <c r="N16">
+        <v>2.15608430732</v>
+      </c>
+      <c r="O16">
         <v>1.9617840104399999</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>3.2035202785500001</v>
       </c>
       <c r="Q16">
@@ -4161,9 +4248,12 @@
         <v>2.01136264856</v>
       </c>
       <c r="N17">
+        <v>0.48564320520699999</v>
+      </c>
+      <c r="O17">
         <v>1.0665333861899999</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>3.6063666701899999</v>
       </c>
       <c r="Q17">
@@ -4250,9 +4340,12 @@
         <v>1.72825671335</v>
       </c>
       <c r="N18">
+        <v>0.983387941228</v>
+      </c>
+      <c r="O18">
         <v>1.22936403886</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>3.6719553577599999</v>
       </c>
       <c r="Q18">
@@ -4339,9 +4432,12 @@
         <v>1.80238201145</v>
       </c>
       <c r="N19">
+        <v>0.30142432336000002</v>
+      </c>
+      <c r="O19">
         <v>1.31968877806</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>3.5240378039400002</v>
       </c>
       <c r="Q19">
@@ -4428,9 +4524,12 @@
         <v>2.7413970706100002</v>
       </c>
       <c r="N20">
+        <v>1.2329170621200001</v>
+      </c>
+      <c r="O20">
         <v>1.2328090195999999</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>3.5162278200200001</v>
       </c>
       <c r="Q20">
@@ -4517,9 +4616,12 @@
         <v>2.53030312959</v>
       </c>
       <c r="N21">
+        <v>1.0473158846799999</v>
+      </c>
+      <c r="O21">
         <v>1.36595250887</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>3.5835439079400002</v>
       </c>
       <c r="Q21">
@@ -4606,9 +4708,12 @@
         <v>2.2823570134</v>
       </c>
       <c r="N22">
+        <v>0.79761894902899999</v>
+      </c>
+      <c r="O22">
         <v>1.46525050842</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>3.6519659234100001</v>
       </c>
       <c r="Q22">
@@ -4695,9 +4800,12 @@
         <v>3.0298532146300001</v>
       </c>
       <c r="N23">
+        <v>2.3798844832600001</v>
+      </c>
+      <c r="O23">
         <v>1.91214875248</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>3.5651451162600001</v>
       </c>
       <c r="Q23">
@@ -4784,9 +4892,12 @@
         <v>3.20453121668</v>
       </c>
       <c r="N24">
+        <v>3.1076502128599999</v>
+      </c>
+      <c r="O24">
         <v>2.06787862905</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>3.74182563408</v>
       </c>
       <c r="Q24">
@@ -4873,9 +4984,12 @@
         <v>2.50589555029</v>
       </c>
       <c r="N25">
+        <v>2.42062857123</v>
+      </c>
+      <c r="O25">
         <v>1.98854342411</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>3.78030694481</v>
       </c>
       <c r="Q25">
@@ -4962,9 +5076,12 @@
         <v>2.3674936933100001</v>
       </c>
       <c r="N26">
+        <v>0.61603486916399997</v>
+      </c>
+      <c r="O26">
         <v>1.5734254515599999</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>4.1661033747299996</v>
       </c>
       <c r="Q26">
@@ -5051,9 +5168,12 @@
         <v>2.4363731783599998</v>
       </c>
       <c r="N27">
+        <v>0.22207112487899999</v>
+      </c>
+      <c r="O27">
         <v>1.6319462203099999</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>3.9592162677</v>
       </c>
       <c r="Q27">
@@ -5140,9 +5260,12 @@
         <v>2.3153524883299998</v>
       </c>
       <c r="N28">
+        <v>0.10751685016</v>
+      </c>
+      <c r="O28">
         <v>1.4252587077400001</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>3.9963360007199999</v>
       </c>
       <c r="Q28">
@@ -5229,9 +5352,12 @@
         <v>3.5942658821900002</v>
       </c>
       <c r="N29">
+        <v>1.50631299666</v>
+      </c>
+      <c r="O29">
         <v>1.61590021889</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>4.0391184541399996</v>
       </c>
       <c r="Q29">
@@ -5318,9 +5444,12 @@
         <v>3.50255149406</v>
       </c>
       <c r="N30">
+        <v>1.18006168118</v>
+      </c>
+      <c r="O30">
         <v>1.5550071588700001</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>4.1105748710099999</v>
       </c>
       <c r="Q30">
@@ -5407,9 +5536,12 @@
         <v>3.2189747532099999</v>
       </c>
       <c r="N31">
+        <v>0.69987706014600004</v>
+      </c>
+      <c r="O31">
         <v>1.39486620152</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>4.05292287313</v>
       </c>
       <c r="Q31">
@@ -5496,9 +5628,12 @@
         <v>3.71305717597</v>
       </c>
       <c r="N32">
+        <v>2.7922339151700002</v>
+      </c>
+      <c r="O32">
         <v>2.0590505185699999</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>3.9779361693999999</v>
       </c>
       <c r="Q32">
@@ -5585,9 +5720,12 @@
         <v>3.5369972660600002</v>
       </c>
       <c r="N33">
+        <v>2.8272644063999999</v>
+      </c>
+      <c r="O33">
         <v>1.84333635323</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>4.2137764580799999</v>
       </c>
       <c r="Q33">
@@ -5665,10 +5803,14 @@
       </c>
       <c r="N34">
         <f>AVERAGE(N8:N33)</f>
-        <v>1.5895465053830766</v>
+        <v>1.3041405299119617</v>
       </c>
       <c r="O34">
         <f>AVERAGE(O8:O33)</f>
+        <v>1.5895465053830766</v>
+      </c>
+      <c r="P34">
+        <f>AVERAGE(P8:P33)</f>
         <v>3.6315450856473079</v>
       </c>
       <c r="T34">
@@ -5738,10 +5880,14 @@
       </c>
       <c r="N35">
         <f>STDEV(N8:N34)</f>
-        <v>0.34336825990440234</v>
+        <v>0.87745416307340185</v>
       </c>
       <c r="O35">
         <f>STDEV(O8:O34)</f>
+        <v>0.34336825990440234</v>
+      </c>
+      <c r="P35">
+        <f>STDEV(P8:P34)</f>
         <v>0.34949856973957899</v>
       </c>
       <c r="T35">
@@ -5802,9 +5948,12 @@
         <v>17</v>
       </c>
       <c r="N39" t="s">
+        <v>20</v>
+      </c>
+      <c r="O39" t="s">
         <v>18</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>19</v>
       </c>
       <c r="T39" s="1" t="s">
@@ -5861,9 +6010,12 @@
         <v>2.3596503588273077</v>
       </c>
       <c r="N40">
+        <v>1.3041405299119617</v>
+      </c>
+      <c r="O40">
         <v>1.5895465053830766</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <v>3.6315450856473079</v>
       </c>
       <c r="S40" t="s">
@@ -5926,9 +6078,12 @@
         <v>0.78322806625704622</v>
       </c>
       <c r="N41">
+        <v>0.87745416307340185</v>
+      </c>
+      <c r="O41">
         <v>0.34336825990440234</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>0.34949856973957899</v>
       </c>
       <c r="S41" t="s">

</xml_diff>